<commit_message>
Netzreglerberechnungen für Leitungen hinzugefügt
</commit_message>
<xml_diff>
--- a/data/Leitungstabelle.xlsx
+++ b/data/Leitungstabelle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F350926-B292-FD4E-A54B-DA300981343C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35C4FB4-92F0-A748-B6BA-8461B5D1FE58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="260" yWindow="480" windowWidth="28240" windowHeight="16220" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Erlaubnis Vorgabe Bemessungsleistung oPL</t>
   </si>
   <si>
-    <t>aktuelle Leistung pL [in %]</t>
+    <t xml:space="preserve">aktuelle Leistung pL </t>
   </si>
 </sst>
 </file>
@@ -127,12 +127,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,14 +512,14 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>15*D2</f>
-        <v>450</v>
+        <v>1425</v>
       </c>
       <c r="G2">
         <v>33</v>
@@ -539,7 +545,7 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F9" si="0">15*D3</f>
@@ -569,7 +575,7 @@
         <v>50</v>
       </c>
       <c r="E4">
-        <v>70</v>
+        <v>-0.7</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -599,7 +605,7 @@
         <v>70</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -629,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -659,7 +665,7 @@
         <v>100</v>
       </c>
       <c r="E7">
-        <v>60</v>
+        <v>-0.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -686,14 +692,14 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>0.3</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="G8">
         <v>33</v>
@@ -742,8 +748,18 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H13" s="3"/>
     </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="L20" s="2"/>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Optimizer ausgebaut und Leitungstabelle von 2010 und Kw_L_Sp-Tabelle von 2050 mit 2 Speichern eingefügt
</commit_message>
<xml_diff>
--- a/data/Leitungstabelle.xlsx
+++ b/data/Leitungstabelle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E729226-FFFA-9148-B276-20940FD2EE49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B68A7-518C-2B45-ADEB-CB4B5D575FDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16260" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="0" yWindow="1320" windowWidth="28800" windowHeight="10960" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Leitungstabelle" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00_ ;\-0.00\ "/>
+    <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -122,10 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -441,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,8 +506,8 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
-        <v>700000</v>
+      <c r="D2" s="5">
+        <v>516150</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -513,7 +517,7 @@
       </c>
       <c r="G2">
         <f>F2*D2</f>
-        <v>4432719.2560000001</v>
+        <v>3268497.2056920002</v>
       </c>
       <c r="H2">
         <v>33</v>
@@ -535,8 +539,8 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
-        <v>700000</v>
+      <c r="D3" s="5">
+        <v>497900</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -546,7 +550,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G10" si="0">F3*D3</f>
-        <v>4173080.3968000002</v>
+        <v>2968252.4708096003</v>
       </c>
       <c r="H3">
         <v>33</v>
@@ -568,8 +572,8 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
-        <v>700000</v>
+      <c r="D4" s="5">
+        <v>493631</v>
       </c>
       <c r="E4">
         <v>-0.7</v>
@@ -579,7 +583,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>3600069.4436000003</v>
+        <v>2538722.6850195881</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -601,8 +605,8 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
-        <v>700000</v>
+      <c r="D5" s="5">
+        <v>485976.92328059423</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -612,7 +616,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>4102023.8909999998</v>
+        <v>2847841.3568166737</v>
       </c>
       <c r="H5">
         <v>33</v>
@@ -634,8 +638,8 @@
       <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
-        <v>700000</v>
+      <c r="D6" s="5">
+        <v>500010</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -645,7 +649,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>3759853.7206999999</v>
+        <v>2685663.5126960101</v>
       </c>
       <c r="H6">
         <v>33</v>
@@ -667,8 +671,8 @@
       <c r="C7">
         <v>7</v>
       </c>
-      <c r="D7" s="2">
-        <v>700000</v>
+      <c r="D7" s="5">
+        <v>100010</v>
       </c>
       <c r="E7">
         <v>-0.6</v>
@@ -678,7 +682,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>3402028.8064000001</v>
+        <v>486052.71561151999</v>
       </c>
       <c r="H7">
         <v>33</v>
@@ -700,8 +704,8 @@
       <c r="C8">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>700000</v>
+      <c r="D8" s="5">
+        <v>536700</v>
       </c>
       <c r="E8">
         <v>0.3</v>
@@ -711,7 +715,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3242745.7503</v>
+        <v>2486259.4916943</v>
       </c>
       <c r="H8">
         <v>33</v>
@@ -733,8 +737,8 @@
       <c r="C9">
         <v>9</v>
       </c>
-      <c r="D9" s="2">
-        <v>700000</v>
+      <c r="D9" s="5">
+        <v>213310</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -744,7 +748,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3806481.3149999999</v>
+        <v>1159943.6132894999</v>
       </c>
       <c r="H9">
         <v>33</v>
@@ -766,8 +770,8 @@
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" s="2">
-        <v>700000</v>
+      <c r="D10" s="5">
+        <v>213310</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -777,7 +781,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4352401.6360999998</v>
+        <v>1326301.1328521301</v>
       </c>
       <c r="H10">
         <v>33</v>
@@ -788,6 +792,51 @@
       <c r="J10">
         <v>1</v>
       </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>